<commit_message>
dev board: fix wrong parts on BOM
</commit_message>
<xml_diff>
--- a/dev_board/bom.xlsx
+++ b/dev_board/bom.xlsx
@@ -125,7 +125,7 @@
     <t xml:space="preserve">J4</t>
   </si>
   <si>
-    <t xml:space="preserve">2057-2PH1-08-UA-SMT-B-ND</t>
+    <t xml:space="preserve"> A122210-ND</t>
   </si>
   <si>
     <t xml:space="preserve">01x08 2.54mm pin header (Probe Connector)</t>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">J5</t>
   </si>
   <si>
-    <t xml:space="preserve">609-54202-G0804LF-ND</t>
+    <t xml:space="preserve"> 609-3486-2-ND</t>
   </si>
   <si>
     <t xml:space="preserve">02x08 2.54mm SMD pin header (Jumper terminal)</t>
@@ -385,10 +385,10 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.9"/>

</xml_diff>

<commit_message>
dev board: add RXMPU 1K pullup resistor to BOM
</commit_message>
<xml_diff>
--- a/dev_board/bom.xlsx
+++ b/dev_board/bom.xlsx
@@ -176,7 +176,7 @@
     <t xml:space="preserve">12K</t>
   </si>
   <si>
-    <t xml:space="preserve">R6, R13</t>
+    <t xml:space="preserve">R6, R13, R15</t>
   </si>
   <si>
     <t xml:space="preserve">2019-RK73H2ATTD1001FTR-ND</t>
@@ -385,10 +385,10 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.9"/>
@@ -629,7 +629,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>51</v>

</xml_diff>